<commit_message>
x3tc/T2D: new validators, new structure version, refactoring (WIP)
</commit_message>
<xml_diff>
--- a/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
+++ b/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
@@ -488,7 +488,39 @@
             <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
-Значение интерпретируется по-разному, в зависимости от типа структуры</t>
+Интерпретируется в зависимости от типа структуры
+Для ShipStruct.SpecReserve допустимо:
+1) указать ware что бы получить размер резерва. Если не зарезервирован, то вернет 0
+2) не указывать, тогда вернет массив товаров, для которых есть записи</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E93" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Шалмеев Дмитрий:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+Значение интерпретируется по-разному, в зависимости от типа структуры
+Для ShipStruct.SpecReserve допустимо:
+Задать резерв: arg3=ware arg4=количество
+</t>
         </r>
       </text>
     </comment>
@@ -497,7 +529,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="259">
   <si>
     <t>descr</t>
   </si>
@@ -1093,18 +1125,6 @@
     <t>Вывести в лог сообщение боевого журнала, при условии что для корабля включено журналирование и установлен глобальный флаг журналирование боевых событий.</t>
   </si>
   <si>
-    <t>Проверить, что аргумент является библиотечной (T2-Droid) структурой данных указанного типа.</t>
-  </si>
-  <si>
-    <t>Строковый идентификатор типа структуры: WareStruct, WorkspaceStruct, etc…</t>
-  </si>
-  <si>
-    <t>TRUE, если аргумент является структурой указанного типа.</t>
-  </si>
-  <si>
-    <t>Аргумент для проверки</t>
-  </si>
-  <si>
     <t>Шаблон формата сообщения, текст или text-id шаблона (см. 591)</t>
   </si>
   <si>
@@ -1265,6 +1285,27 @@
   </si>
   <si>
     <t>Получить количество товара в трюме с учетом всех резервов (например, батареи за вычетом резерва под ПД)</t>
+  </si>
+  <si>
+    <t>Доп. значение (опционально, см. arg3)</t>
+  </si>
+  <si>
+    <t>Получить конфиг корабля</t>
+  </si>
+  <si>
+    <t>ShipStruct</t>
+  </si>
+  <si>
+    <t>Ship (опционально, если не указан, то используется THIS)</t>
+  </si>
+  <si>
+    <t>Элемент массива или null в случае ошибки</t>
+  </si>
+  <si>
+    <t>Ключ (опционально)</t>
+  </si>
+  <si>
+    <t>Получить данные поля-массива</t>
   </si>
 </sst>
 </file>
@@ -3403,11 +3444,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J112"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I61" sqref="I61"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J92" sqref="J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3423,7 +3464,7 @@
     <col min="9" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3449,7 +3490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -3475,18 +3516,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>198</v>
+        <v>253</v>
       </c>
       <c r="B3" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>201</v>
+        <v>255</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>199</v>
+        <v>10</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>10</v>
@@ -3498,11 +3539,10 @@
         <v>10</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="J3" s="37"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -3528,7 +3568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -3554,7 +3594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
@@ -3580,7 +3620,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -3606,7 +3646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
@@ -3632,7 +3672,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
@@ -3658,7 +3698,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
@@ -3684,7 +3724,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>36</v>
       </c>
@@ -3710,7 +3750,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>180</v>
       </c>
@@ -3736,7 +3776,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>41</v>
       </c>
@@ -3762,7 +3802,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>44</v>
       </c>
@@ -3788,7 +3828,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>49</v>
       </c>
@@ -3814,7 +3854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>54</v>
       </c>
@@ -3863,7 +3903,7 @@
         <v>10</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -4476,7 +4516,7 @@
         <v>592</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>111</v>
@@ -4529,7 +4569,7 @@
         <v>594</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>111</v>
@@ -4616,7 +4656,7 @@
     </row>
     <row r="47" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B47" s="7">
         <v>598</v>
@@ -4643,13 +4683,13 @@
     </row>
     <row r="48" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B48" s="7">
         <v>599</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>111</v>
@@ -4686,7 +4726,7 @@
         <v>601</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D50" s="25" t="s">
         <v>10</v>
@@ -4701,7 +4741,7 @@
         <v>10</v>
       </c>
       <c r="H50" s="25" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="J50" s="37"/>
     </row>
@@ -4909,7 +4949,7 @@
     </row>
     <row r="61" spans="1:10" s="27" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="25" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B61" s="26">
         <v>609</v>
@@ -5403,7 +5443,7 @@
         <v>163</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G80" s="34" t="s">
         <v>10</v>
@@ -5412,7 +5452,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>164</v>
       </c>
@@ -5438,7 +5478,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>169</v>
       </c>
@@ -5464,7 +5504,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>171</v>
       </c>
@@ -5490,9 +5530,9 @@
         <v>173</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B84" s="7">
         <v>705</v>
@@ -5513,10 +5553,10 @@
         <v>10</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="6"/>
       <c r="B85" s="7"/>
       <c r="C85" s="6"/>
@@ -5526,7 +5566,7 @@
       <c r="G85" s="6"/>
       <c r="H85" s="6"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="6"/>
       <c r="B86" s="7"/>
       <c r="C86" s="6"/>
@@ -5536,9 +5576,9 @@
       <c r="G86" s="6"/>
       <c r="H86" s="6"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="39" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B87" s="40"/>
       <c r="C87" s="40"/>
@@ -5548,15 +5588,15 @@
       <c r="G87" s="40"/>
       <c r="H87" s="41"/>
     </row>
-    <row r="88" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B88" s="7">
         <v>8200</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>10</v>
@@ -5571,21 +5611,21 @@
         <v>10</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B89" s="7">
         <v>8201</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>10</v>
@@ -5597,24 +5637,24 @@
         <v>10</v>
       </c>
       <c r="H89" s="6" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="42" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B90" s="43">
         <v>8202</v>
       </c>
       <c r="C90" s="44" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D90" s="44" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E90" s="44" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F90" s="44" t="s">
         <v>10</v>
@@ -5623,153 +5663,154 @@
         <v>10</v>
       </c>
       <c r="H90" s="45" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="42" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B91" s="43">
         <v>8203</v>
       </c>
       <c r="C91" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="D91" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="E91" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F91" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G91" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H91" s="45" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="B92" s="43">
+        <v>8210</v>
+      </c>
+      <c r="C92" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="D92" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="E92" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="F92" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G92" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H92" s="45" t="s">
+        <v>256</v>
+      </c>
+      <c r="J92" s="37"/>
+    </row>
+    <row r="93" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="B93" s="43">
+        <v>8211</v>
+      </c>
+      <c r="C93" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="D93" s="44" t="s">
+        <v>216</v>
+      </c>
+      <c r="E93" s="44" t="s">
         <v>217</v>
       </c>
-      <c r="D91" s="44" t="s">
-        <v>235</v>
-      </c>
-      <c r="E91" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="F91" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G91" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H91" s="45" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="42" t="s">
+      <c r="F93" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="G93" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" s="45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="B94" s="43">
+        <v>8212</v>
+      </c>
+      <c r="C94" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="D94" s="44" t="s">
+        <v>216</v>
+      </c>
+      <c r="E94" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="B92" s="43">
-        <v>8211</v>
-      </c>
-      <c r="C92" s="44" t="s">
-        <v>217</v>
-      </c>
-      <c r="D92" s="44" t="s">
+      <c r="F94" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G94" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" s="45" t="s">
         <v>220</v>
       </c>
-      <c r="E92" s="44" t="s">
-        <v>221</v>
-      </c>
-      <c r="F92" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G92" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H92" s="45" t="s">
+    </row>
+    <row r="95" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="42" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="42" t="s">
-        <v>232</v>
-      </c>
-      <c r="B93" s="43">
-        <v>8212</v>
-      </c>
-      <c r="C93" s="44" t="s">
-        <v>217</v>
-      </c>
-      <c r="D93" s="44" t="s">
-        <v>220</v>
-      </c>
-      <c r="E93" s="44" t="s">
+      <c r="B95" s="43">
+        <v>8213</v>
+      </c>
+      <c r="C95" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="D95" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="F93" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G93" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H93" s="45" t="s">
+      <c r="E95" s="44" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="42" t="s">
-        <v>226</v>
-      </c>
-      <c r="B94" s="43">
-        <v>8213</v>
-      </c>
-      <c r="C94" s="44" t="s">
-        <v>217</v>
-      </c>
-      <c r="D94" s="44" t="s">
-        <v>227</v>
-      </c>
-      <c r="E94" s="44" t="s">
-        <v>228</v>
-      </c>
-      <c r="F94" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G94" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" s="45" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="42" t="s">
-        <v>237</v>
-      </c>
-      <c r="B95" s="43">
+      <c r="F95" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G95" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H95" s="45" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="B96" s="43">
         <v>8214</v>
       </c>
-      <c r="C95" s="44" t="s">
-        <v>217</v>
-      </c>
-      <c r="D95" s="44" t="s">
-        <v>227</v>
-      </c>
-      <c r="E95" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="F95" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G95" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H95" s="45" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="42" t="s">
-        <v>246</v>
-      </c>
-      <c r="B96" s="43">
-        <v>8215</v>
-      </c>
       <c r="C96" s="44" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
       <c r="D96" s="44" t="s">
-        <v>227</v>
-      </c>
-      <c r="E96" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="E96" s="44" t="s">
         <v>10</v>
       </c>
       <c r="F96" s="44" t="s">
@@ -5779,24 +5820,24 @@
         <v>10</v>
       </c>
       <c r="H96" s="45" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="42" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B97" s="43">
-        <v>8221</v>
+        <v>8215</v>
       </c>
       <c r="C97" s="44" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="D97" s="44" t="s">
-        <v>230</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>241</v>
+        <v>223</v>
+      </c>
+      <c r="E97" s="46" t="s">
+        <v>10</v>
       </c>
       <c r="F97" s="44" t="s">
         <v>10</v>
@@ -5805,24 +5846,24 @@
         <v>10</v>
       </c>
       <c r="H97" s="45" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="42" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B98" s="43">
-        <v>8222</v>
+        <v>8221</v>
       </c>
       <c r="C98" s="44" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D98" s="44" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F98" s="44" t="s">
         <v>10</v>
@@ -5831,44 +5872,60 @@
         <v>10</v>
       </c>
       <c r="H98" s="45" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="42" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B99" s="43">
+        <v>8222</v>
+      </c>
+      <c r="C99" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="D99" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F99" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G99" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H99" s="45" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="42" t="s">
+        <v>238</v>
+      </c>
+      <c r="B100" s="43">
         <v>8223</v>
       </c>
-      <c r="C99" s="44" t="s">
-        <v>217</v>
-      </c>
-      <c r="D99" s="44" t="s">
-        <v>230</v>
-      </c>
-      <c r="E99" s="44" t="s">
-        <v>243</v>
-      </c>
-      <c r="F99" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G99" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H99" s="45" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="42"/>
-      <c r="B100" s="43"/>
-      <c r="C100" s="44"/>
-      <c r="D100" s="44"/>
-      <c r="E100" s="44"/>
-      <c r="F100" s="44"/>
-      <c r="G100" s="44"/>
-      <c r="H100" s="45"/>
+      <c r="C100" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="D100" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="E100" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="F100" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G100" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H100" s="45" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="42"/>
@@ -5881,64 +5938,64 @@
       <c r="H101" s="45"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="39" t="s">
-        <v>207</v>
-      </c>
-      <c r="B102" s="40"/>
-      <c r="C102" s="40"/>
-      <c r="D102" s="40"/>
-      <c r="E102" s="40"/>
-      <c r="F102" s="40"/>
-      <c r="G102" s="40"/>
-      <c r="H102" s="41"/>
+      <c r="A102" s="42"/>
+      <c r="B102" s="43"/>
+      <c r="C102" s="44"/>
+      <c r="D102" s="44"/>
+      <c r="E102" s="44"/>
+      <c r="F102" s="44"/>
+      <c r="G102" s="44"/>
+      <c r="H102" s="45"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="6"/>
-      <c r="B103" s="7">
+      <c r="A103" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="B103" s="40"/>
+      <c r="C103" s="40"/>
+      <c r="D103" s="40"/>
+      <c r="E103" s="40"/>
+      <c r="F103" s="40"/>
+      <c r="G103" s="40"/>
+      <c r="H103" s="41"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="6"/>
+      <c r="B104" s="7">
         <v>11200</v>
       </c>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
-      <c r="F103" s="6"/>
-      <c r="G103" s="6"/>
-      <c r="H103" s="6"/>
-    </row>
-    <row r="104" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A104" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="B104" s="7">
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+    </row>
+    <row r="105" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A105" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B105" s="7">
         <v>11201</v>
       </c>
-      <c r="C104" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="D104" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E104" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F104" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G104" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H104" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="6"/>
-      <c r="B105" s="7"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
-      <c r="H105" s="6"/>
+      <c r="C105" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H105" s="6" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="6"/>
@@ -6010,9 +6067,19 @@
       <c r="G112" s="6"/>
       <c r="H112" s="6"/>
     </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="6"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A102:H102"/>
+    <mergeCell ref="A103:H103"/>
     <mergeCell ref="A87:H87"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
x3tc/T2D: new validators implemented, refactoring (WIP)
</commit_message>
<xml_diff>
--- a/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
+++ b/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
@@ -22,7 +22,7 @@
     <author>Шалмеев Дмитрий</author>
   </authors>
   <commentList>
-    <comment ref="D11" authorId="0">
+    <comment ref="D13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -35,7 +35,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0">
+    <comment ref="C21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,34 @@
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0">
+    <comment ref="J21" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Шалмеев Дмитрий:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+На удалении
+Замена - 8200</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0">
+    <comment ref="D23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -80,7 +107,34 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0">
+    <comment ref="J23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Шалмеев Дмитрий:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+На удаление
+Замена 8204</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0">
+    <comment ref="E24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0">
+    <comment ref="A25" authorId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C29" authorId="0">
+    <comment ref="C31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D29" authorId="0">
+    <comment ref="D31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -145,7 +199,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H29" authorId="0">
+    <comment ref="H31" authorId="0">
       <text>
         <r>
           <rPr>
@@ -162,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D34" authorId="0">
+    <comment ref="D36" authorId="0">
       <text>
         <r>
           <rPr>
@@ -178,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="0">
+    <comment ref="A39" authorId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A38" authorId="0">
+    <comment ref="A40" authorId="0">
       <text>
         <r>
           <rPr>
@@ -204,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B44" authorId="0">
+    <comment ref="B46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -217,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A50" authorId="0">
+    <comment ref="A52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -230,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A53" authorId="0">
+    <comment ref="A55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -243,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H53" authorId="0">
+    <comment ref="H55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -256,7 +310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A54" authorId="0">
+    <comment ref="A56" authorId="0">
       <text>
         <r>
           <rPr>
@@ -269,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H54" authorId="0">
+    <comment ref="H56" authorId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A61" authorId="0">
+    <comment ref="A63" authorId="0">
       <text>
         <r>
           <rPr>
@@ -295,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C64" authorId="0">
+    <comment ref="C66" authorId="0">
       <text>
         <r>
           <rPr>
@@ -308,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F64" authorId="0">
+    <comment ref="F66" authorId="0">
       <text>
         <r>
           <rPr>
@@ -322,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C65" authorId="0">
+    <comment ref="C67" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F65" authorId="0">
+    <comment ref="F67" authorId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0">
+    <comment ref="A68" authorId="0">
       <text>
         <r>
           <rPr>
@@ -362,7 +416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A67" authorId="0">
+    <comment ref="A69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -375,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A69" authorId="1">
+    <comment ref="A71" authorId="1">
       <text>
         <r>
           <rPr>
@@ -401,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H71" authorId="0">
+    <comment ref="H73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -414,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A73" authorId="0">
+    <comment ref="A75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -427,7 +481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A74" authorId="0">
+    <comment ref="A76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -440,7 +494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A75" authorId="0">
+    <comment ref="A77" authorId="0">
       <text>
         <r>
           <rPr>
@@ -453,7 +507,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A76" authorId="0">
+    <comment ref="A78" authorId="0">
       <text>
         <r>
           <rPr>
@@ -466,7 +520,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E92" authorId="1">
+    <comment ref="E95" authorId="1">
       <text>
         <r>
           <rPr>
@@ -495,7 +549,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E93" authorId="1">
+    <comment ref="E96" authorId="1">
       <text>
         <r>
           <rPr>
@@ -529,7 +583,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="269">
   <si>
     <t>descr</t>
   </si>
@@ -1306,6 +1360,36 @@
   </si>
   <si>
     <t>Получить данные поля-массива</t>
+  </si>
+  <si>
+    <t>Скопировать данные структуры или создать новую копию</t>
+  </si>
+  <si>
+    <t>Экземпляр целевой структуры (опционально, если не указан, то создается новая копия)</t>
+  </si>
+  <si>
+    <t>Экземпляр исходной структуры</t>
+  </si>
+  <si>
+    <t>Экземпяр со скопированными данными или null в случае ошибки</t>
+  </si>
+  <si>
+    <t>Сравнить два массива рекурсивно</t>
+  </si>
+  <si>
+    <t>TRUE если массивы равны</t>
+  </si>
+  <si>
+    <t>Массив 1</t>
+  </si>
+  <si>
+    <t>Массив 2</t>
+  </si>
+  <si>
+    <t>Проверить, являются ли аргументы одинаковыми копиями или это один и тот же экземпляр массива. Проверка выполняется рекурсивно. Все вложенные массивы так же должны быть копиями, а не ссылками на один массив.</t>
+  </si>
+  <si>
+    <t>TRUE если аргументы являются полными копиями и не содержат ссылки на общие массивы</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1435,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1368,12 +1452,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9966"/>
         <bgColor rgb="FFFF99CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF94BD5E"/>
-        <bgColor rgb="FFAECF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -1440,6 +1518,18 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor rgb="FFAECF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1533,7 +1623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1581,13 +1671,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1609,33 +1699,17 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1651,6 +1725,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1745,7 +1842,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1788,7 +1885,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1831,7 +1928,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1874,7 +1971,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1917,7 +2014,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1960,7 +2057,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2003,7 +2100,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2046,7 +2143,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2089,7 +2186,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2132,7 +2229,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2175,7 +2272,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2218,7 +2315,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2261,7 +2358,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2304,7 +2401,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2347,7 +2444,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2390,7 +2487,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2433,7 +2530,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2476,7 +2573,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2519,7 +2616,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2562,7 +2659,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2605,7 +2702,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2648,7 +2745,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2691,7 +2788,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2734,7 +2831,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2777,7 +2874,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2820,7 +2917,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2863,7 +2960,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2906,7 +3003,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2949,7 +3046,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2992,7 +3089,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3035,7 +3132,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3078,7 +3175,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3121,7 +3218,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3444,11 +3541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J92" sqref="J92"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3464,7 +3561,7 @@
     <col min="9" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3490,7 +3587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -3516,7 +3613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>253</v>
       </c>
@@ -3542,142 +3639,144 @@
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" s="7">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="J4" s="34"/>
+    </row>
+    <row r="5" spans="1:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B5" s="7">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="J5" s="34"/>
+    </row>
+    <row r="6" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B6" s="7">
         <v>51</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="7" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B7" s="7">
         <v>52</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="6" t="s">
+      <c r="D7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B8" s="7">
         <v>53</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="D8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="9" spans="1:10" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B9" s="7">
         <v>54</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="7">
-        <v>55</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="7">
-        <v>56</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>21</v>
@@ -3686,443 +3785,443 @@
         <v>22</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="H9" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="7">
+        <v>55</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="7">
+        <v>56</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B12" s="7">
         <v>57</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="6" t="s">
+      <c r="D12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="13" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B13" s="7">
         <v>58</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="6" t="s">
+      <c r="F13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B14" s="7">
         <v>59</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D12" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="6" t="s">
+      <c r="D14" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="15" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B15" s="7">
         <v>500</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="D15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="16" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B16" s="7">
         <v>501</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="6" t="s">
+      <c r="F16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="17" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B17" s="7">
         <v>502</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="G17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B18" s="7">
         <v>503</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="6" t="s">
+      <c r="G18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="19" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B19" s="7">
         <v>504</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="C19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+    <row r="20" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B20" s="7">
         <v>505</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="C20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+    <row r="21" spans="1:10" s="49" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B21" s="48">
         <v>506</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C21" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="9" t="s">
+      <c r="D21" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="47" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+    <row r="22" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B22" s="7">
         <v>507</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="6" t="s">
+      <c r="G22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+    <row r="23" spans="1:10" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B23" s="45">
         <v>508</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C23" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D23" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="6" t="s">
+      <c r="E23" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="44" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+    <row r="24" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B24" s="7">
         <v>509</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="6" t="s">
+      <c r="F24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+    <row r="25" spans="1:10" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B25" s="10">
         <v>510</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C25" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="12" t="s">
+      <c r="D25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="7">
-        <v>511</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="7">
-        <v>512</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B26" s="7">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>10</v>
@@ -4137,439 +4236,438 @@
         <v>10</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="7">
+        <v>512</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="7">
+        <v>513</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B29" s="7">
         <v>514</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="6" t="s">
+      <c r="D29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+    <row r="30" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B30" s="7">
         <v>515</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="C30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B31" s="7">
         <v>516</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H29" s="6" t="s">
+      <c r="E31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+    <row r="32" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B32" s="7">
         <v>517</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="6" t="s">
+      <c r="E32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="J30" s="37"/>
-    </row>
-    <row r="31" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+      <c r="J32" s="34"/>
+    </row>
+    <row r="33" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B33" s="7">
         <v>518</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="6" t="s">
+      <c r="F33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="J31" s="37"/>
-    </row>
-    <row r="32" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+      <c r="J33" s="34"/>
+    </row>
+    <row r="34" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B34" s="7">
         <v>519</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="6" t="s">
+      <c r="E34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="J32" s="37"/>
-    </row>
-    <row r="33" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="J34" s="34"/>
+    </row>
+    <row r="35" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B35" s="7">
         <v>520</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="6" t="s">
+      <c r="D35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="J33" s="37"/>
-    </row>
-    <row r="34" spans="1:10" s="17" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
+      <c r="J35" s="34"/>
+    </row>
+    <row r="36" spans="1:10" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B36" s="13">
         <v>530</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C36" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D36" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
+      <c r="E36" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B37" s="7">
         <v>531</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="6" t="s">
+      <c r="D37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="20" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
+    <row r="38" spans="1:10" s="17" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="19">
+      <c r="B38" s="16">
         <v>532</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C38" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D38" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E38" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F38" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="G36" s="18" t="s">
+      <c r="G38" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H38" s="15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
+    <row r="39" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B39" s="7">
         <v>533</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E39" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F39" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H37" s="6" t="s">
+      <c r="G39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="21" t="s">
+    <row r="40" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B40" s="7">
         <v>534</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E40" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="H40" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
+    <row r="41" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B41" s="7">
         <v>590</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C41" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D41" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E41" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F41" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="G39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="24" customFormat="1" ht="177.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="22" t="s">
+      <c r="G41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="21" customFormat="1" ht="177.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="23">
+      <c r="B42" s="20">
         <v>591</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C42" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D42" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E42" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F42" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="G40" s="22" t="s">
+      <c r="G42" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="H40" s="22" t="s">
+      <c r="H42" s="19" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+    <row r="43" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B43" s="7">
         <v>592</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J41" s="37"/>
-    </row>
-    <row r="42" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B42" s="7">
-        <v>593</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="7">
-        <v>594</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>198</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>111</v>
@@ -4586,31 +4684,43 @@
       <c r="H43" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J43" s="37"/>
-    </row>
-    <row r="44" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="J43" s="34"/>
+    </row>
+    <row r="44" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B44" s="7">
-        <v>595</v>
-      </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-    </row>
-    <row r="45" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>593</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="B45" s="7">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>111</v>
@@ -4627,39 +4737,28 @@
       <c r="H45" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J45" s="34"/>
+    </row>
+    <row r="46" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>197</v>
+        <v>119</v>
       </c>
       <c r="B46" s="7">
-        <v>597</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>595</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="B47" s="7">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>175</v>
@@ -4679,17 +4778,16 @@
       <c r="H47" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J47" s="38"/>
-    </row>
-    <row r="48" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B48" s="7">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>111</v>
@@ -4706,1310 +4804,1344 @@
       <c r="H48" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J48" s="37"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="6"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-    </row>
-    <row r="50" spans="1:10" s="27" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="25" t="s">
+    </row>
+    <row r="49" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B49" s="7">
+        <v>598</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J49" s="35"/>
+    </row>
+    <row r="50" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B50" s="7">
+        <v>599</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J50" s="34"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="6"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:10" s="24" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="B50" s="26">
+      <c r="B52" s="23">
         <v>601</v>
       </c>
-      <c r="C50" s="25" t="s">
+      <c r="C52" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="D50" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="25" t="s">
+      <c r="D52" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H52" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="J50" s="37"/>
-    </row>
-    <row r="51" spans="1:10" s="27" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="25" t="s">
+      <c r="J52" s="34"/>
+    </row>
+    <row r="53" spans="1:10" s="24" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="B51" s="26">
+      <c r="B53" s="23">
         <v>602</v>
       </c>
-      <c r="C51" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G51" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H51" s="25" t="s">
+      <c r="C53" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H53" s="22" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="27" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A52" s="25" t="s">
+    <row r="54" spans="1:10" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A54" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="B52" s="26">
+      <c r="B54" s="23">
         <v>603</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C54" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="D52" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G52" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H52" s="25" t="s">
+      <c r="D54" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H54" s="22" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="27" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A53" s="25" t="s">
+    <row r="55" spans="1:10" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A55" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="B53" s="26">
+      <c r="B55" s="23">
         <v>604</v>
       </c>
-      <c r="C53" s="25" t="s">
+      <c r="C55" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D53" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G53" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H53" s="25" t="s">
+      <c r="D55" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H55" s="22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A54" s="25" t="s">
+    <row r="56" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A56" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="B54" s="26">
+      <c r="B56" s="23">
         <v>605</v>
       </c>
-      <c r="C54" s="25" t="s">
+      <c r="C56" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D54" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G54" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H54" s="25" t="s">
+      <c r="D56" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H56" s="22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A55" s="25" t="s">
+    <row r="57" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A57" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="B55" s="26">
+      <c r="B57" s="23">
         <v>606</v>
       </c>
-      <c r="C55" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G55" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H55" s="25" t="s">
+      <c r="C57" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H57" s="22" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="D56"/>
-      <c r="E56"/>
-      <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56"/>
-    </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="6"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-    </row>
-    <row r="59" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="25" t="s">
+      <c r="A58"/>
+      <c r="B58"/>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="6"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="B59" s="26">
+      <c r="B61" s="23">
         <v>607</v>
       </c>
-      <c r="C59" s="25" t="s">
+      <c r="C61" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="D59" s="25" t="s">
+      <c r="D61" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="E59" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F59" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G59" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H59" s="25" t="s">
+      <c r="E61" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H61" s="22" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="25" t="s">
+    <row r="62" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B60" s="26">
+      <c r="B62" s="23">
         <v>608</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C62" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="D60" s="25" t="s">
+      <c r="D62" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="E60" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F60" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G60" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H60" s="25" t="s">
+      <c r="E62" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H62" s="22" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="27" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="25" t="s">
+    <row r="63" spans="1:10" s="24" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="B61" s="26">
+      <c r="B63" s="23">
         <v>609</v>
       </c>
-      <c r="C61" s="25" t="s">
+      <c r="C63" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D61" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F61" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G61" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H61" s="25" t="s">
+      <c r="D63" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H63" s="22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-      <c r="F62"/>
-      <c r="G62"/>
-      <c r="H62"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64"/>
+      <c r="B64"/>
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64"/>
+      <c r="H64"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B65" s="7">
         <v>610</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C65" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D65" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="E63" s="6" t="s">
+      <c r="E65" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F63" s="6" t="s">
+      <c r="F65" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G63" s="6" t="s">
+      <c r="G65" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="H63" s="6" t="s">
+      <c r="H65" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
+    <row r="66" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B64" s="7">
+      <c r="B66" s="7">
         <v>611</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C66" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D66" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="E66" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F64" s="6" t="s">
+      <c r="F66" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G64" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H64" s="6" t="s">
+      <c r="G66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H66" s="6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="30" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A65" s="28" t="s">
+    <row r="67" spans="1:10" s="27" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A67" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="B65" s="29">
+      <c r="B67" s="26">
         <v>612</v>
       </c>
-      <c r="C65" s="28" t="s">
+      <c r="C67" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="D65" s="28" t="s">
+      <c r="D67" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="E65" s="28" t="s">
+      <c r="E67" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="F65" s="28" t="s">
+      <c r="F67" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G65" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="H65" s="28" t="s">
+      <c r="G67" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H67" s="25" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="27" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A66" s="25" t="s">
+    <row r="68" spans="1:10" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A68" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="B66" s="26">
+      <c r="B68" s="23">
         <v>613</v>
       </c>
-      <c r="C66" s="25" t="s">
+      <c r="C68" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D66" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F66" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G66" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H66" s="25" t="s">
+      <c r="D68" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H68" s="22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
+    <row r="69" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B67" s="7">
+      <c r="B69" s="7">
         <v>614</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C69" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D67" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H67" s="6" t="s">
+      <c r="D69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H69" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="31" t="s">
+    <row r="70" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="B68" s="32">
+      <c r="B70" s="29">
         <v>615</v>
       </c>
-      <c r="C68" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F68" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="G68" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="H68" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A69" s="36" t="s">
+      <c r="C70" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G70" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H70" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A71" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B71" s="7">
         <v>616</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J69" s="38"/>
-    </row>
-    <row r="70" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
+      <c r="C71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J71" s="35"/>
+    </row>
+    <row r="72" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A72" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B70" s="7">
+      <c r="B72" s="7">
         <v>617</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G70" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
+      <c r="C72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A73" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B73" s="7">
         <v>618</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C73" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D73" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="E71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H71" s="6" t="s">
+      <c r="E73" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H73" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
+    <row r="74" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B72" s="7">
+      <c r="B74" s="7">
         <v>619</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C74" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D72" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G72" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H72" s="6" t="s">
+      <c r="D74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H74" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B75" s="7">
         <v>620</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C75" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H73" s="6" t="s">
+      <c r="D75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H75" s="6" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
+    <row r="76" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A76" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B74" s="7">
+      <c r="B76" s="7">
         <v>621</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C76" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="D74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H74" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
+      <c r="D76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A77" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B75" s="7">
+      <c r="B77" s="7">
         <v>622</v>
       </c>
-      <c r="C75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
+      <c r="C77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A78" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B76" s="7">
+      <c r="B78" s="7">
         <v>623</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C78" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H76" s="6" t="s">
+      <c r="D78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H78" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
+    <row r="79" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B79" s="7">
         <v>624</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C79" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D77" s="6" t="s">
+      <c r="D79" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="E77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H77" s="6" t="s">
+      <c r="E79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H79" s="6" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
+    <row r="80" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A80" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="B78" s="7">
+      <c r="B80" s="7">
         <v>625</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C80" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H78" s="6" t="s">
+      <c r="D80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H80" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B79" s="7">
+      <c r="B81" s="7">
         <v>700</v>
       </c>
-      <c r="C79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H79" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B80" s="7">
-        <v>701</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="G80" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H80" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B81" s="7">
-        <v>702</v>
-      </c>
       <c r="C81" s="6" t="s">
-        <v>165</v>
+        <v>10</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>166</v>
+        <v>10</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>167</v>
+        <v>10</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="G81" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G81" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H81" s="6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" ht="153" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B82" s="7">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="G82" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="G82" s="31" t="s">
         <v>10</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="7">
+        <v>702</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G83" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H83" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A84" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B84" s="7">
+        <v>703</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G84" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B85" s="7">
         <v>704</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="D83" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H83" s="6" t="s">
+      <c r="D85" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H85" s="6" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A84" s="6" t="s">
+    <row r="86" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A86" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="B84" s="7">
+      <c r="B86" s="7">
         <v>705</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C86" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="D84" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H84" s="6" t="s">
+      <c r="D86" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H86" s="6" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A85" s="6"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="6"/>
-      <c r="G85" s="6"/>
-      <c r="H85" s="6"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A86" s="6"/>
-      <c r="B86" s="7"/>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="6"/>
-      <c r="F86" s="6"/>
-      <c r="G86" s="6"/>
-      <c r="H86" s="6"/>
-    </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A87" s="39" t="s">
+      <c r="A87" s="6"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" s="6"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="B87" s="40"/>
-      <c r="C87" s="40"/>
-      <c r="D87" s="40"/>
-      <c r="E87" s="40"/>
-      <c r="F87" s="40"/>
-      <c r="G87" s="40"/>
-      <c r="H87" s="41"/>
-    </row>
-    <row r="88" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="6" t="s">
+      <c r="B89" s="42"/>
+      <c r="C89" s="42"/>
+      <c r="D89" s="42"/>
+      <c r="E89" s="42"/>
+      <c r="F89" s="42"/>
+      <c r="G89" s="42"/>
+      <c r="H89" s="43"/>
+    </row>
+    <row r="90" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B88" s="7">
+      <c r="B90" s="7">
         <v>8200</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C90" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D88" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F88" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G88" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H88" s="6" t="s">
+      <c r="D90" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G90" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H90" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="6" t="s">
+    <row r="91" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B89" s="7">
+      <c r="B91" s="7">
         <v>8201</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C91" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="D91" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="E89" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H89" s="6" t="s">
+      <c r="E91" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G91" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H91" s="6" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="42" t="s">
+    <row r="92" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="B90" s="43">
+      <c r="B92" s="37">
         <v>8202</v>
       </c>
-      <c r="C90" s="44" t="s">
+      <c r="C92" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D90" s="44" t="s">
+      <c r="D92" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="E90" s="44" t="s">
+      <c r="E92" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="F90" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G90" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H90" s="45" t="s">
+      <c r="F92" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G92" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H92" s="39" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="42" t="s">
+    <row r="93" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="B91" s="43">
+      <c r="B93" s="37">
         <v>8203</v>
       </c>
-      <c r="C91" s="44" t="s">
+      <c r="C93" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D91" s="44" t="s">
+      <c r="D93" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="E91" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="F91" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G91" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H91" s="45" t="s">
+      <c r="E93" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F93" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G93" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" s="39" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="42" t="s">
+    <row r="94" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="B94" s="37">
+        <v>8204</v>
+      </c>
+      <c r="C94" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D94" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="E94" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F94" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G94" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" s="39" t="s">
+        <v>262</v>
+      </c>
+      <c r="J94" s="34"/>
+    </row>
+    <row r="95" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="36" t="s">
         <v>258</v>
       </c>
-      <c r="B92" s="43">
+      <c r="B95" s="37">
         <v>8210</v>
       </c>
-      <c r="C92" s="44" t="s">
+      <c r="C95" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D92" s="44" t="s">
+      <c r="D95" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="E92" s="44" t="s">
+      <c r="E95" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="F92" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G92" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H92" s="45" t="s">
+      <c r="F95" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G95" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H95" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="J92" s="37"/>
-    </row>
-    <row r="93" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="42" t="s">
+      <c r="J95" s="34"/>
+    </row>
+    <row r="96" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="36" t="s">
         <v>215</v>
       </c>
-      <c r="B93" s="43">
+      <c r="B96" s="37">
         <v>8211</v>
       </c>
-      <c r="C93" s="44" t="s">
+      <c r="C96" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D93" s="44" t="s">
+      <c r="D96" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="E93" s="44" t="s">
+      <c r="E96" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="F93" s="44" t="s">
+      <c r="F96" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="G93" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H93" s="45" t="s">
+      <c r="G96" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H96" s="39" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="42" t="s">
+    <row r="97" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="B94" s="43">
+      <c r="B97" s="37">
         <v>8212</v>
       </c>
-      <c r="C94" s="44" t="s">
+      <c r="C97" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D94" s="44" t="s">
+      <c r="D97" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="E94" s="44" t="s">
+      <c r="E97" s="38" t="s">
         <v>219</v>
       </c>
-      <c r="F94" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G94" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" s="45" t="s">
+      <c r="F97" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G97" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H97" s="39" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="42" t="s">
+    <row r="98" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="B95" s="43">
+      <c r="B98" s="37">
         <v>8213</v>
       </c>
-      <c r="C95" s="44" t="s">
+      <c r="C98" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D95" s="44" t="s">
+      <c r="D98" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="E95" s="44" t="s">
+      <c r="E98" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="F95" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G95" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H95" s="45" t="s">
+      <c r="F98" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G98" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H98" s="39" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="42" t="s">
+    <row r="99" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="36" t="s">
         <v>233</v>
       </c>
-      <c r="B96" s="43">
+      <c r="B99" s="37">
         <v>8214</v>
       </c>
-      <c r="C96" s="44" t="s">
+      <c r="C99" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D96" s="44" t="s">
+      <c r="D99" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="E96" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="F96" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G96" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H96" s="45" t="s">
+      <c r="E99" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G99" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H99" s="39" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="42" t="s">
+    <row r="100" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="36" t="s">
         <v>242</v>
       </c>
-      <c r="B97" s="43">
+      <c r="B100" s="37">
         <v>8215</v>
       </c>
-      <c r="C97" s="44" t="s">
+      <c r="C100" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="D97" s="44" t="s">
+      <c r="D100" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="E97" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="F97" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G97" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H97" s="45" t="s">
+      <c r="E100" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F100" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G100" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H100" s="39" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="42" t="s">
+    <row r="101" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="36" t="s">
         <v>244</v>
       </c>
-      <c r="B98" s="43">
+      <c r="B101" s="37">
         <v>8221</v>
       </c>
-      <c r="C98" s="44" t="s">
+      <c r="C101" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D98" s="44" t="s">
+      <c r="D101" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="E101" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="F98" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G98" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H98" s="45" t="s">
+      <c r="F101" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G101" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H101" s="39" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="42" t="s">
+    <row r="102" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="36" t="s">
         <v>235</v>
       </c>
-      <c r="B99" s="43">
+      <c r="B102" s="37">
         <v>8222</v>
       </c>
-      <c r="C99" s="44" t="s">
+      <c r="C102" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D99" s="44" t="s">
+      <c r="D102" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="E102" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="F99" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G99" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H99" s="45" t="s">
+      <c r="F102" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G102" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H102" s="39" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="42" t="s">
+    <row r="103" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="36" t="s">
         <v>238</v>
       </c>
-      <c r="B100" s="43">
+      <c r="B103" s="37">
         <v>8223</v>
       </c>
-      <c r="C100" s="44" t="s">
+      <c r="C103" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="D100" s="44" t="s">
+      <c r="D103" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="E100" s="44" t="s">
+      <c r="E103" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="F100" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G100" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H100" s="45" t="s">
+      <c r="F103" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G103" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H103" s="39" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="42"/>
-      <c r="B101" s="43"/>
-      <c r="C101" s="44"/>
-      <c r="D101" s="44"/>
-      <c r="E101" s="44"/>
-      <c r="F101" s="44"/>
-      <c r="G101" s="44"/>
-      <c r="H101" s="45"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="42"/>
-      <c r="B102" s="43"/>
-      <c r="C102" s="44"/>
-      <c r="D102" s="44"/>
-      <c r="E102" s="44"/>
-      <c r="F102" s="44"/>
-      <c r="G102" s="44"/>
-      <c r="H102" s="45"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="39" t="s">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="36"/>
+      <c r="B104" s="37"/>
+      <c r="C104" s="38"/>
+      <c r="D104" s="38"/>
+      <c r="E104" s="38"/>
+      <c r="F104" s="38"/>
+      <c r="G104" s="38"/>
+      <c r="H104" s="39"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="36"/>
+      <c r="B105" s="37"/>
+      <c r="C105" s="38"/>
+      <c r="D105" s="38"/>
+      <c r="E105" s="38"/>
+      <c r="F105" s="38"/>
+      <c r="G105" s="38"/>
+      <c r="H105" s="39"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="B103" s="40"/>
-      <c r="C103" s="40"/>
-      <c r="D103" s="40"/>
-      <c r="E103" s="40"/>
-      <c r="F103" s="40"/>
-      <c r="G103" s="40"/>
-      <c r="H103" s="41"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="6"/>
-      <c r="B104" s="7">
-        <v>11200</v>
-      </c>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
-      <c r="F104" s="6"/>
-      <c r="G104" s="6"/>
-      <c r="H104" s="6"/>
-    </row>
-    <row r="105" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A105" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="B105" s="7">
-        <v>11201</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E105" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H105" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="6"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-      <c r="E106" s="6"/>
-      <c r="F106" s="6"/>
-      <c r="G106" s="6"/>
-      <c r="H106" s="6"/>
+      <c r="B106" s="42"/>
+      <c r="C106" s="42"/>
+      <c r="D106" s="42"/>
+      <c r="E106" s="42"/>
+      <c r="F106" s="42"/>
+      <c r="G106" s="42"/>
+      <c r="H106" s="43"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="6"/>
-      <c r="B107" s="7"/>
+      <c r="B107" s="7">
+        <v>11200</v>
+      </c>
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
       <c r="E107" s="6"/>
@@ -6017,15 +6149,31 @@
       <c r="G107" s="6"/>
       <c r="H107" s="6"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="6"/>
-      <c r="B108" s="7"/>
-      <c r="C108" s="6"/>
-      <c r="D108" s="6"/>
-      <c r="E108" s="6"/>
-      <c r="F108" s="6"/>
-      <c r="G108" s="6"/>
-      <c r="H108" s="6"/>
+    <row r="108" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A108" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B108" s="7">
+        <v>11201</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G108" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H108" s="6" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="6"/>
@@ -6077,10 +6225,40 @@
       <c r="G113" s="6"/>
       <c r="H113" s="6"/>
     </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="6"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="6"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="6"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A103:H103"/>
-    <mergeCell ref="A87:H87"/>
+    <mergeCell ref="A106:H106"/>
+    <mergeCell ref="A89:H89"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
x3tc/T2D: scripts switched to new validation
</commit_message>
<xml_diff>
--- a/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
+++ b/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
@@ -258,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="0">
+    <comment ref="B47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -583,7 +583,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="270">
   <si>
     <t>descr</t>
   </si>
@@ -1390,6 +1390,9 @@
   </si>
   <si>
     <t>TRUE если аргументы являются полными копиями и не содержат ссылки на общие массивы</t>
+  </si>
+  <si>
+    <t>Вывести в лог сообщение валидатора при условии, что для корабля включено журналирование и установлен глобальный флаг журнала валидации.</t>
   </si>
 </sst>
 </file>
@@ -1725,15 +1728,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1748,6 +1742,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -3544,8 +3547,8 @@
   <dimension ref="A1:J116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3875,7 +3878,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>36</v>
       </c>
@@ -4083,29 +4086,29 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="49" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="47" t="s">
+    <row r="21" spans="1:10" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="48">
+      <c r="B21" s="45">
         <v>506</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="47" t="s">
+      <c r="D21" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="44" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4135,29 +4138,29 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="44" t="s">
+    <row r="23" spans="1:10" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="45">
+      <c r="B23" s="42">
         <v>508</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="44" t="s">
+      <c r="E23" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="41" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4607,184 +4610,184 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B41" s="7">
+        <v>589</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B42" s="7">
         <v>590</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="G41" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" s="21" customFormat="1" ht="177.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="19" t="s">
+      <c r="G42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="21" customFormat="1" ht="177.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="B42" s="20">
+      <c r="B43" s="20">
         <v>591</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C43" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D43" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="E43" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="F42" s="19" t="s">
+      <c r="F43" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="G42" s="19" t="s">
+      <c r="G43" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="H42" s="19" t="s">
+      <c r="H43" s="19" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+    <row r="44" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B44" s="7">
         <v>592</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H43" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J43" s="34"/>
-    </row>
-    <row r="44" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+      <c r="H44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J44" s="34"/>
+    </row>
+    <row r="45" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B45" s="7">
         <v>593</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H44" s="6" t="s">
+      <c r="C45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
+    <row r="46" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B46" s="7">
         <v>594</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E46" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F46" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="G46" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H45" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J45" s="34"/>
-    </row>
-    <row r="46" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+      <c r="H46" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J46" s="34"/>
+    </row>
+    <row r="47" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B47" s="7">
         <v>595</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-    </row>
-    <row r="47" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B48" s="7">
         <v>596</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B48" s="7">
-        <v>597</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>175</v>
@@ -4807,10 +4810,10 @@
     </row>
     <row r="49" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B49" s="7">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>175</v>
@@ -4830,17 +4833,16 @@
       <c r="H49" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J49" s="35"/>
-    </row>
-    <row r="50" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B50" s="7">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>111</v>
@@ -4857,17 +4859,34 @@
       <c r="H50" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J50" s="34"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
+      <c r="J50" s="35"/>
+    </row>
+    <row r="51" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B51" s="7">
+        <v>599</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J51" s="34"/>
     </row>
     <row r="52" spans="1:10" s="24" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
@@ -5728,16 +5747,16 @@
       <c r="H88" s="6"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A89" s="41" t="s">
+      <c r="A89" s="47" t="s">
         <v>207</v>
       </c>
-      <c r="B89" s="42"/>
-      <c r="C89" s="42"/>
-      <c r="D89" s="42"/>
-      <c r="E89" s="42"/>
-      <c r="F89" s="42"/>
-      <c r="G89" s="42"/>
-      <c r="H89" s="43"/>
+      <c r="B89" s="48"/>
+      <c r="C89" s="48"/>
+      <c r="D89" s="48"/>
+      <c r="E89" s="48"/>
+      <c r="F89" s="48"/>
+      <c r="G89" s="48"/>
+      <c r="H89" s="49"/>
     </row>
     <row r="90" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
@@ -6126,16 +6145,16 @@
       <c r="H105" s="39"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="41" t="s">
+      <c r="A106" s="47" t="s">
         <v>203</v>
       </c>
-      <c r="B106" s="42"/>
-      <c r="C106" s="42"/>
-      <c r="D106" s="42"/>
-      <c r="E106" s="42"/>
-      <c r="F106" s="42"/>
-      <c r="G106" s="42"/>
-      <c r="H106" s="43"/>
+      <c r="B106" s="48"/>
+      <c r="C106" s="48"/>
+      <c r="D106" s="48"/>
+      <c r="E106" s="48"/>
+      <c r="F106" s="48"/>
+      <c r="G106" s="48"/>
+      <c r="H106" s="49"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="6"/>

</xml_diff>

<commit_message>
x3tc/T2D: function 611 tested and refactored
</commit_message>
<xml_diff>
--- a/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
+++ b/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
@@ -22,7 +22,7 @@
     <author>Шалмеев Дмитрий</author>
   </authors>
   <commentList>
-    <comment ref="D15" authorId="0">
+    <comment ref="D16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -35,7 +35,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C23" authorId="0">
+    <comment ref="C24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J23" authorId="1">
+    <comment ref="J24" authorId="1">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0">
+    <comment ref="A26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D25" authorId="0">
+    <comment ref="D26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="1">
+    <comment ref="J26" authorId="1">
       <text>
         <r>
           <rPr>
@@ -134,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C26" authorId="0">
+    <comment ref="C27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E26" authorId="0">
+    <comment ref="E27" authorId="0">
       <text>
         <r>
           <rPr>
@@ -160,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0">
+    <comment ref="A28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C33" authorId="0">
+    <comment ref="C34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -186,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D33" authorId="0">
+    <comment ref="D34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -199,7 +199,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H33" authorId="0">
+    <comment ref="H34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -216,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D38" authorId="0">
+    <comment ref="D39" authorId="0">
       <text>
         <r>
           <rPr>
@@ -229,19 +229,6 @@
 1 - копировать параметры рабочей области
 2 - копировать список товаров
 По умолчанию копируется все</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A41" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Еще используется?</t>
         </r>
       </text>
     </comment>
@@ -258,7 +245,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B49" authorId="0">
+    <comment ref="A43" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Еще используется?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B50" authorId="0">
       <text>
         <r>
           <rPr>
@@ -271,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A54" authorId="0">
+    <comment ref="A55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -284,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A57" authorId="0">
+    <comment ref="A58" authorId="0">
       <text>
         <r>
           <rPr>
@@ -297,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H57" authorId="0">
+    <comment ref="H58" authorId="0">
       <text>
         <r>
           <rPr>
@@ -310,7 +310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A58" authorId="0">
+    <comment ref="A59" authorId="0">
       <text>
         <r>
           <rPr>
@@ -323,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H58" authorId="0">
+    <comment ref="H59" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A65" authorId="0">
+    <comment ref="A66" authorId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C68" authorId="0">
+    <comment ref="C69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -362,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F68" authorId="0">
+    <comment ref="F69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -376,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C69" authorId="0">
+    <comment ref="C70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -390,7 +390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F69" authorId="0">
+    <comment ref="F70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -403,7 +403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A70" authorId="0">
+    <comment ref="A71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -416,7 +416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A71" authorId="0">
+    <comment ref="A72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -429,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A73" authorId="1">
+    <comment ref="A74" authorId="1">
       <text>
         <r>
           <rPr>
@@ -455,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H75" authorId="0">
+    <comment ref="H76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -468,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A77" authorId="0">
+    <comment ref="A78" authorId="0">
       <text>
         <r>
           <rPr>
@@ -481,7 +481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A78" authorId="0">
+    <comment ref="A79" authorId="0">
       <text>
         <r>
           <rPr>
@@ -494,7 +494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A79" authorId="0">
+    <comment ref="A80" authorId="0">
       <text>
         <r>
           <rPr>
@@ -507,7 +507,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A80" authorId="0">
+    <comment ref="A81" authorId="0">
       <text>
         <r>
           <rPr>
@@ -520,7 +520,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E97" authorId="1">
+    <comment ref="E98" authorId="1">
       <text>
         <r>
           <rPr>
@@ -549,7 +549,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E98" authorId="1">
+    <comment ref="E99" authorId="1">
       <text>
         <r>
           <rPr>
@@ -583,7 +583,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="276">
   <si>
     <t>descr</t>
   </si>
@@ -1402,6 +1402,15 @@
   </si>
   <si>
     <t>Новый массив</t>
+  </si>
+  <si>
+    <t>Проверить, что первый массив содержит все элементы второго без учета порядка.</t>
+  </si>
+  <si>
+    <t>Массив1</t>
+  </si>
+  <si>
+    <t>TRUE, если в первом массиве есть все элементы второго</t>
   </si>
 </sst>
 </file>
@@ -1861,7 +1870,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1904,7 +1913,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1947,7 +1956,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1990,7 +1999,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2033,7 +2042,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2076,7 +2085,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2119,7 +2128,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2162,7 +2171,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2205,7 +2214,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2248,7 +2257,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2291,7 +2300,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2334,7 +2343,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2377,7 +2386,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2420,7 +2429,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2463,7 +2472,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2506,7 +2515,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2549,7 +2558,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2592,7 +2601,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2635,7 +2644,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2678,7 +2687,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2721,7 +2730,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2764,7 +2773,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2807,7 +2816,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2850,7 +2859,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2893,7 +2902,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2936,7 +2945,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2979,7 +2988,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3022,7 +3031,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3065,7 +3074,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3108,7 +3117,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3151,7 +3160,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3194,7 +3203,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3237,7 +3246,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1247775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3560,11 +3569,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J67" sqref="J67"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3766,324 +3775,325 @@
       </c>
       <c r="J7" s="34"/>
     </row>
-    <row r="8" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" s="7">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="J8" s="34"/>
+    </row>
+    <row r="9" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B9" s="7">
         <v>51</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="6" t="s">
+      <c r="C9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="7">
-        <v>52</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="7">
+        <v>52</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B11" s="7">
         <v>53</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="6" t="s">
+      <c r="D11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="12" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B12" s="7">
         <v>54</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="13" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B13" s="7">
         <v>55</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="6" t="s">
+      <c r="E13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="B13" s="7">
-        <v>56</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B14" s="7">
+        <v>56</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B15" s="7">
         <v>57</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="6" t="s">
+      <c r="D15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="16" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B16" s="7">
         <v>58</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="F16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B16" s="7">
-        <v>59</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D16" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="7">
+        <v>59</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B18" s="7">
         <v>500</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="D18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+    <row r="19" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B19" s="7">
         <v>501</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="F19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="7">
-        <v>502</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B20" s="7">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>49</v>
@@ -4092,7 +4102,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>52</v>
@@ -4101,226 +4111,226 @@
         <v>10</v>
       </c>
       <c r="H20" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="7">
+        <v>503</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+    <row r="22" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B22" s="7">
         <v>504</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="6" t="s">
+      <c r="C22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B23" s="7">
         <v>505</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="6" t="s">
+      <c r="C23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="44" t="s">
+    <row r="24" spans="1:10" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="45">
+      <c r="B24" s="45">
         <v>506</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C24" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="44" t="s">
+      <c r="D24" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="44" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+    <row r="25" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B25" s="7">
         <v>507</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="6" t="s">
+      <c r="G25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="41" t="s">
+    <row r="26" spans="1:10" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="42">
+      <c r="B26" s="42">
         <v>508</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C26" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="41" t="s">
+      <c r="D26" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="41" t="s">
+      <c r="E26" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="41" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+    <row r="27" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B27" s="7">
         <v>509</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="6" t="s">
+      <c r="F27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+    <row r="28" spans="1:10" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B28" s="10">
         <v>510</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="9" t="s">
+      <c r="D28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" s="7">
-        <v>511</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B29" s="7">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>10</v>
@@ -4340,10 +4350,10 @@
     </row>
     <row r="30" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="7">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>10</v>
@@ -4361,180 +4371,179 @@
         <v>10</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="7">
+        <v>513</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B32" s="7">
         <v>514</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="6" t="s">
+      <c r="D32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="7">
-        <v>515</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="7">
+        <v>515</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B34" s="7">
         <v>516</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="6" t="s">
+      <c r="E34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+    <row r="35" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B35" s="7">
         <v>517</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H34" s="6" t="s">
+      <c r="E35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="J34" s="34"/>
-    </row>
-    <row r="35" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="B35" s="7">
-        <v>518</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="J35" s="34"/>
     </row>
     <row r="36" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B36" s="7">
+        <v>518</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J36" s="34"/>
+    </row>
+    <row r="37" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B37" s="7">
         <v>519</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="J36" s="34"/>
-    </row>
-    <row r="37" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B37" s="7">
-        <v>520</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>190</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>10</v>
+        <v>191</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>10</v>
@@ -4546,120 +4555,121 @@
         <v>10</v>
       </c>
       <c r="H37" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="J37" s="34"/>
+    </row>
+    <row r="38" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B38" s="7">
+        <v>520</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="J37" s="34"/>
-    </row>
-    <row r="38" spans="1:10" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
+      <c r="J38" s="34"/>
+    </row>
+    <row r="39" spans="1:10" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B38" s="13">
+      <c r="B39" s="13">
         <v>530</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C39" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D39" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E38" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
+      <c r="E39" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B40" s="7">
         <v>531</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H39" s="6" t="s">
+      <c r="D40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="17" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="15" t="s">
+    <row r="41" spans="1:10" s="17" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B40" s="16">
+      <c r="B41" s="16">
         <v>532</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C41" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D41" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E41" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F41" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="G41" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="H40" s="15" t="s">
+      <c r="H41" s="15" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="7">
-        <v>533</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B42" s="7">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>97</v>
@@ -4671,219 +4681,219 @@
         <v>93</v>
       </c>
       <c r="F42" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="7">
+        <v>534</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="G43" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H42" s="6" t="s">
+      <c r="H43" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+    <row r="44" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B44" s="7">
         <v>589</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H43" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+      <c r="H44" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B45" s="7">
         <v>590</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E45" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="F45" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" s="21" customFormat="1" ht="177.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="19" t="s">
+      <c r="G45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="21" customFormat="1" ht="177.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="20">
+      <c r="B46" s="20">
         <v>591</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C46" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D46" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E45" s="19" t="s">
+      <c r="E46" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F45" s="19" t="s">
+      <c r="F46" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="G45" s="19" t="s">
+      <c r="G46" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="H45" s="19" t="s">
+      <c r="H46" s="19" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+    <row r="47" spans="1:10" ht="123" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B47" s="7">
         <v>592</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="G47" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H46" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J46" s="34"/>
-    </row>
-    <row r="47" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+      <c r="H47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J47" s="34"/>
+    </row>
+    <row r="48" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B48" s="7">
         <v>593</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H47" s="6" t="s">
+      <c r="C48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H48" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+    <row r="49" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B49" s="7">
         <v>594</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E49" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F49" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="G49" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H48" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J48" s="34"/>
-    </row>
-    <row r="49" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
+      <c r="H49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J49" s="34"/>
+    </row>
+    <row r="50" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B50" s="7">
         <v>595</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-    </row>
-    <row r="50" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B51" s="7">
         <v>596</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B51" s="7">
-        <v>597</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>174</v>
@@ -4906,10 +4916,10 @@
     </row>
     <row r="52" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B52" s="7">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>174</v>
@@ -4929,17 +4939,16 @@
       <c r="H52" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J52" s="35"/>
-    </row>
-    <row r="53" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B53" s="7">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>110</v>
@@ -4956,70 +4965,71 @@
       <c r="H53" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J53" s="34"/>
-    </row>
-    <row r="54" spans="1:10" s="24" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="22" t="s">
+      <c r="J53" s="35"/>
+    </row>
+    <row r="54" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B54" s="7">
+        <v>599</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J54" s="34"/>
+    </row>
+    <row r="55" spans="1:10" s="24" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="23">
+      <c r="B55" s="23">
         <v>601</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C55" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="D54" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G54" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H54" s="22" t="s">
+      <c r="D55" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H55" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="J54" s="34"/>
-    </row>
-    <row r="55" spans="1:10" s="24" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="22" t="s">
+      <c r="J55" s="34"/>
+    </row>
+    <row r="56" spans="1:10" s="24" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="B55" s="23">
+      <c r="B56" s="23">
         <v>602</v>
       </c>
-      <c r="C55" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G55" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H55" s="22" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A56" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B56" s="23">
-        <v>603</v>
-      </c>
       <c r="C56" s="22" t="s">
-        <v>123</v>
+        <v>10</v>
       </c>
       <c r="D56" s="22" t="s">
         <v>10</v>
@@ -5039,37 +5049,36 @@
     </row>
     <row r="57" spans="1:10" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A57" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" s="23">
+        <v>603</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H57" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" s="24" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A58" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B57" s="23">
+      <c r="B58" s="23">
         <v>604</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E57" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F57" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G57" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H57" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="J57" s="50"/>
-    </row>
-    <row r="58" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A58" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="B58" s="23">
-        <v>605</v>
       </c>
       <c r="C58" s="22" t="s">
         <v>125</v>
@@ -5089,87 +5098,88 @@
       <c r="H58" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="J58" s="35"/>
-    </row>
-    <row r="59" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="J58" s="50"/>
+    </row>
+    <row r="59" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A59" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B59" s="23">
+        <v>605</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G59" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H59" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="J59" s="35"/>
+    </row>
+    <row r="60" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A60" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="B59" s="23">
+      <c r="B60" s="23">
         <v>606</v>
       </c>
-      <c r="C59" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F59" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G59" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H59" s="22" t="s">
+      <c r="C60" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G60" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H60" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="J59" s="35"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" s="6"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-      <c r="H62" s="6"/>
-    </row>
-    <row r="63" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="B63" s="23">
-        <v>607</v>
-      </c>
-      <c r="C63" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="D63" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="E63" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F63" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G63" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H63" s="22" t="s">
-        <v>132</v>
-      </c>
+      <c r="J60" s="35"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="6"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
     </row>
     <row r="64" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="22" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B64" s="23">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C64" s="22" t="s">
         <v>130</v>
@@ -5190,80 +5200,80 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="24" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B65" s="23">
+        <v>608</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H65" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" s="24" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="B65" s="23">
+      <c r="B66" s="23">
         <v>609</v>
       </c>
-      <c r="C65" s="22" t="s">
+      <c r="C66" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D65" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F65" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G65" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H65" s="22" t="s">
+      <c r="D66" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H66" s="22" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A66"/>
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="D66"/>
-      <c r="E66"/>
-      <c r="F66"/>
-      <c r="G66"/>
-      <c r="H66"/>
-    </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
+      <c r="A67"/>
+      <c r="B67"/>
+      <c r="C67"/>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="G67"/>
+      <c r="H67"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B67" s="7">
+      <c r="B68" s="7">
         <v>610</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H67" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B68" s="7">
-        <v>611</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>135</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>125</v>
@@ -5272,207 +5282,207 @@
         <v>138</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>10</v>
+        <v>130</v>
       </c>
       <c r="H68" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" s="7">
+        <v>611</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H69" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="27" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A69" s="25" t="s">
+    <row r="70" spans="1:10" s="27" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A70" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="B69" s="26">
+      <c r="B70" s="26">
         <v>612</v>
       </c>
-      <c r="C69" s="25" t="s">
+      <c r="C70" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="D69" s="25" t="s">
+      <c r="D70" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="E69" s="25" t="s">
+      <c r="E70" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="F69" s="25" t="s">
+      <c r="F70" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="G69" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H69" s="25" t="s">
+      <c r="G70" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H70" s="25" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A70" s="22" t="s">
+    <row r="71" spans="1:10" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A71" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="B70" s="23">
+      <c r="B71" s="23">
         <v>613</v>
       </c>
-      <c r="C70" s="22" t="s">
+      <c r="C71" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D70" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F70" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G70" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H70" s="22" t="s">
+      <c r="D71" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H71" s="22" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
+    <row r="72" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A72" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B72" s="7">
         <v>614</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C72" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H71" s="6" t="s">
+      <c r="D72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H72" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="28" t="s">
+    <row r="73" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="B72" s="29">
+      <c r="B73" s="29">
         <v>615</v>
       </c>
-      <c r="C72" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D72" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F72" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G72" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="H72" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A73" s="33" t="s">
+      <c r="C73" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G73" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H73" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A74" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B74" s="7">
         <v>616</v>
       </c>
-      <c r="C73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J73" s="35"/>
-    </row>
-    <row r="74" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
+      <c r="C74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J74" s="35"/>
+    </row>
+    <row r="75" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B74" s="7">
+      <c r="B75" s="7">
         <v>617</v>
       </c>
-      <c r="C74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H74" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
+      <c r="C75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A76" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="7">
+      <c r="B76" s="7">
         <v>618</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B76" s="7">
-        <v>619</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>148</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>10</v>
+        <v>149</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>10</v>
@@ -5487,148 +5497,148 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="7">
+        <v>619</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B78" s="7">
         <v>620</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C78" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H77" s="6" t="s">
+      <c r="D78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H78" s="6" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B78" s="7">
-        <v>621</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H78" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" s="7">
+        <v>621</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A80" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B79" s="7">
+      <c r="B80" s="7">
         <v>622</v>
       </c>
-      <c r="C79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H79" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
+      <c r="C80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A81" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B80" s="7">
+      <c r="B81" s="7">
         <v>623</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C81" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D80" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F80" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H80" s="6" t="s">
+      <c r="D81" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H81" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
+    <row r="82" spans="1:8" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="B81" s="7">
+      <c r="B82" s="7">
         <v>624</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G81" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H81" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B82" s="7">
-        <v>625</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>148</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>10</v>
+        <v>178</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>10</v>
@@ -5640,79 +5650,79 @@
         <v>10</v>
       </c>
       <c r="H82" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A83" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B83" s="7">
+        <v>625</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H83" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A83" s="6" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B84" s="7">
         <v>700</v>
       </c>
-      <c r="C83" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H83" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="A84" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B84" s="7">
-        <v>701</v>
-      </c>
       <c r="C84" s="6" t="s">
-        <v>160</v>
+        <v>10</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>161</v>
+        <v>10</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>162</v>
+        <v>10</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="G84" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G84" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="153" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B85" s="7">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>167</v>
+        <v>245</v>
       </c>
       <c r="G85" s="31" t="s">
         <v>10</v>
@@ -5721,12 +5731,12 @@
         <v>158</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B86" s="7">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>164</v>
@@ -5738,7 +5748,7 @@
         <v>166</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G86" s="31" t="s">
         <v>10</v>
@@ -5747,38 +5757,38 @@
         <v>158</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B87" s="7">
+        <v>703</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="G87" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="B87" s="7">
+      <c r="B88" s="7">
         <v>704</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F87" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G87" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H87" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A88" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B88" s="7">
-        <v>705</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>171</v>
@@ -5796,20 +5806,36 @@
         <v>10</v>
       </c>
       <c r="H88" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A89" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B89" s="7">
+        <v>705</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H89" s="6" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A89" s="6"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="6"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="6"/>
-      <c r="F89" s="6"/>
-      <c r="G89" s="6"/>
-      <c r="H89" s="6"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="6"/>
       <c r="B90" s="7"/>
       <c r="C90" s="6"/>
@@ -5819,208 +5845,192 @@
       <c r="G90" s="6"/>
       <c r="H90" s="6"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A91" s="47" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="6"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="47" t="s">
         <v>206</v>
       </c>
-      <c r="B91" s="48"/>
-      <c r="C91" s="48"/>
-      <c r="D91" s="48"/>
-      <c r="E91" s="48"/>
-      <c r="F91" s="48"/>
-      <c r="G91" s="48"/>
-      <c r="H91" s="49"/>
-    </row>
-    <row r="92" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="6" t="s">
+      <c r="B92" s="48"/>
+      <c r="C92" s="48"/>
+      <c r="D92" s="48"/>
+      <c r="E92" s="48"/>
+      <c r="F92" s="48"/>
+      <c r="G92" s="48"/>
+      <c r="H92" s="49"/>
+    </row>
+    <row r="93" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B92" s="7">
+      <c r="B93" s="7">
         <v>8200</v>
       </c>
-      <c r="C92" s="6" t="s">
+      <c r="C93" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="D92" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F92" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G92" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H92" s="6" t="s">
+      <c r="D93" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" s="6" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="6" t="s">
+    <row r="94" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B93" s="7">
+      <c r="B94" s="7">
         <v>8201</v>
       </c>
-      <c r="C93" s="6" t="s">
+      <c r="C94" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D93" s="6" t="s">
+      <c r="D94" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="E93" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G93" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H93" s="6" t="s">
+      <c r="E94" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="36" t="s">
+    <row r="95" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="B94" s="37">
+      <c r="B95" s="37">
         <v>8202</v>
-      </c>
-      <c r="C94" s="38" t="s">
-        <v>212</v>
-      </c>
-      <c r="D94" s="38" t="s">
-        <v>229</v>
-      </c>
-      <c r="E94" s="38" t="s">
-        <v>209</v>
-      </c>
-      <c r="F94" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G94" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" s="39" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="36" t="s">
-        <v>228</v>
-      </c>
-      <c r="B95" s="37">
-        <v>8203</v>
       </c>
       <c r="C95" s="38" t="s">
         <v>212</v>
       </c>
       <c r="D95" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="E95" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="F95" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G95" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H95" s="39" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="B96" s="37">
+        <v>8203</v>
+      </c>
+      <c r="C96" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="D96" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="E95" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F95" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G95" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="H95" s="39" t="s">
+      <c r="E96" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G96" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H96" s="39" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="36" t="s">
+    <row r="97" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="36" t="s">
         <v>258</v>
       </c>
-      <c r="B96" s="37">
+      <c r="B97" s="37">
         <v>8204</v>
       </c>
-      <c r="C96" s="38" t="s">
+      <c r="C97" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="D96" s="38" t="s">
+      <c r="D97" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="E96" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F96" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G96" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="H96" s="39" t="s">
+      <c r="E97" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G97" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H97" s="39" t="s">
         <v>261</v>
-      </c>
-      <c r="J96" s="34"/>
-    </row>
-    <row r="97" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="B97" s="37">
-        <v>8210</v>
-      </c>
-      <c r="C97" s="38" t="s">
-        <v>212</v>
-      </c>
-      <c r="D97" s="38" t="s">
-        <v>222</v>
-      </c>
-      <c r="E97" s="38" t="s">
-        <v>256</v>
-      </c>
-      <c r="F97" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G97" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="H97" s="39" t="s">
-        <v>255</v>
       </c>
       <c r="J97" s="34"/>
     </row>
     <row r="98" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="36" t="s">
-        <v>214</v>
+        <v>257</v>
       </c>
       <c r="B98" s="37">
-        <v>8211</v>
+        <v>8210</v>
       </c>
       <c r="C98" s="38" t="s">
         <v>212</v>
       </c>
       <c r="D98" s="38" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="E98" s="38" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
       <c r="F98" s="38" t="s">
-        <v>251</v>
+        <v>10</v>
       </c>
       <c r="G98" s="38" t="s">
         <v>10</v>
       </c>
       <c r="H98" s="39" t="s">
-        <v>217</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="J98" s="34"/>
     </row>
     <row r="99" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="36" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="B99" s="37">
-        <v>8212</v>
+        <v>8211</v>
       </c>
       <c r="C99" s="38" t="s">
         <v>212</v>
@@ -6029,33 +6039,33 @@
         <v>215</v>
       </c>
       <c r="E99" s="38" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F99" s="38" t="s">
-        <v>10</v>
+        <v>251</v>
       </c>
       <c r="G99" s="38" t="s">
         <v>10</v>
       </c>
       <c r="H99" s="39" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="36" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B100" s="37">
-        <v>8213</v>
+        <v>8212</v>
       </c>
       <c r="C100" s="38" t="s">
         <v>212</v>
       </c>
       <c r="D100" s="38" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E100" s="38" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F100" s="38" t="s">
         <v>10</v>
@@ -6064,15 +6074,15 @@
         <v>10</v>
       </c>
       <c r="H100" s="39" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="36" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="B101" s="37">
-        <v>8214</v>
+        <v>8213</v>
       </c>
       <c r="C101" s="38" t="s">
         <v>212</v>
@@ -6081,7 +6091,7 @@
         <v>222</v>
       </c>
       <c r="E101" s="38" t="s">
-        <v>10</v>
+        <v>223</v>
       </c>
       <c r="F101" s="38" t="s">
         <v>10</v>
@@ -6090,23 +6100,23 @@
         <v>10</v>
       </c>
       <c r="H101" s="39" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="36" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="B102" s="37">
-        <v>8215</v>
+        <v>8214</v>
       </c>
       <c r="C102" s="38" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="D102" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="E102" s="40" t="s">
+      <c r="E102" s="38" t="s">
         <v>10</v>
       </c>
       <c r="F102" s="38" t="s">
@@ -6116,24 +6126,24 @@
         <v>10</v>
       </c>
       <c r="H102" s="39" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="36" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B103" s="37">
-        <v>8221</v>
+        <v>8215</v>
       </c>
       <c r="C103" s="38" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
       <c r="D103" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
+      </c>
+      <c r="E103" s="40" t="s">
+        <v>10</v>
       </c>
       <c r="F103" s="38" t="s">
         <v>10</v>
@@ -6142,15 +6152,15 @@
         <v>10</v>
       </c>
       <c r="H103" s="39" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="36" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="B104" s="37">
-        <v>8222</v>
+        <v>8221</v>
       </c>
       <c r="C104" s="38" t="s">
         <v>212</v>
@@ -6159,7 +6169,7 @@
         <v>225</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F104" s="38" t="s">
         <v>10</v>
@@ -6173,10 +6183,10 @@
     </row>
     <row r="105" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="36" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B105" s="37">
-        <v>8223</v>
+        <v>8222</v>
       </c>
       <c r="C105" s="38" t="s">
         <v>212</v>
@@ -6184,28 +6194,44 @@
       <c r="D105" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="E105" s="38" t="s">
+      <c r="E105" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F105" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G105" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H105" s="39" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="B106" s="37">
+        <v>8223</v>
+      </c>
+      <c r="C106" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="D106" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="E106" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="F105" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G105" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="H105" s="39" t="s">
+      <c r="F106" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G106" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H106" s="39" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A106" s="36"/>
-      <c r="B106" s="37"/>
-      <c r="C106" s="38"/>
-      <c r="D106" s="38"/>
-      <c r="E106" s="38"/>
-      <c r="F106" s="38"/>
-      <c r="G106" s="38"/>
-      <c r="H106" s="39"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="36"/>
@@ -6218,64 +6244,64 @@
       <c r="H107" s="39"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A108" s="47" t="s">
+      <c r="A108" s="36"/>
+      <c r="B108" s="37"/>
+      <c r="C108" s="38"/>
+      <c r="D108" s="38"/>
+      <c r="E108" s="38"/>
+      <c r="F108" s="38"/>
+      <c r="G108" s="38"/>
+      <c r="H108" s="39"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" s="47" t="s">
         <v>202</v>
       </c>
-      <c r="B108" s="48"/>
-      <c r="C108" s="48"/>
-      <c r="D108" s="48"/>
-      <c r="E108" s="48"/>
-      <c r="F108" s="48"/>
-      <c r="G108" s="48"/>
-      <c r="H108" s="49"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A109" s="6"/>
-      <c r="B109" s="7">
+      <c r="B109" s="48"/>
+      <c r="C109" s="48"/>
+      <c r="D109" s="48"/>
+      <c r="E109" s="48"/>
+      <c r="F109" s="48"/>
+      <c r="G109" s="48"/>
+      <c r="H109" s="49"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" s="6"/>
+      <c r="B110" s="7">
         <v>11200</v>
       </c>
-      <c r="C109" s="6"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="6"/>
-      <c r="F109" s="6"/>
-      <c r="G109" s="6"/>
-      <c r="H109" s="6"/>
-    </row>
-    <row r="110" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A110" s="6" t="s">
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+    </row>
+    <row r="111" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A111" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="B110" s="7">
+      <c r="B111" s="7">
         <v>11201</v>
       </c>
-      <c r="C110" s="6" t="s">
+      <c r="C111" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D110" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E110" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F110" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G110" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H110" s="6" t="s">
+      <c r="D111" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H111" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A111" s="6"/>
-      <c r="B111" s="7"/>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="6"/>
-      <c r="F111" s="6"/>
-      <c r="G111" s="6"/>
-      <c r="H111" s="6"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="6"/>
@@ -6347,10 +6373,20 @@
       <c r="G118" s="6"/>
       <c r="H118" s="6"/>
     </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="6"/>
+      <c r="B119" s="7"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A108:H108"/>
-    <mergeCell ref="A91:H91"/>
+    <mergeCell ref="A109:H109"/>
+    <mergeCell ref="A92:H92"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
x3tc/T2D: function 601 bugfix for case of non-transportable ware
</commit_message>
<xml_diff>
--- a/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
+++ b/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
@@ -349,6 +349,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="F68" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Шалмеев Дмитрий:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+Если не указано, то отключаются некоторые проверки валидаторов (см. Dev Manual)</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C69" authorId="0">
       <text>
         <r>
@@ -359,20 +385,6 @@
             <charset val="1"/>
           </rPr>
           <t>Требует указания типа контрагента для выбора соответствующего списка дополнительных станций.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F69" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Если не указан, то расчитывается соответствующий лимит из WareStruct в зависимости от типа контрагента.
-Укажи -1, если не нужно проверять количество.</t>
         </r>
       </text>
     </comment>
@@ -3572,8 +3584,8 @@
   <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4742,7 +4754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>103</v>
       </c>

</xml_diff>

<commit_message>
T2D: Refactoring and improvements
- all scripts moved back to X3TC MSCI version
- tests of f601 and f706 are adapted to work both for X3TC and X3AP
- WAL option added to ware editing dialog
- function f601 now uses WAL setting
- MTS and MTB parameters are fixed and improved
- functions f604 and f605 improved in respect of WAL setting
- function f609 refactored and supports WareStruct
- functions f613, f608, f607 are refactored
- wwsl.util.loadProduct now uses WareStruct
- wwsl.util.unloadProduct now uses WareStruct
- added launching the drones before emergency jump
- added destination and command descriptors for defensive procedures
- moved to ShipStruct-3.02
- moved to WareStruct-3.02
- trading with dock is fixed and now respects all validators
- all scripts which use validators are checked upvalidators are fixed
</commit_message>
<xml_diff>
--- a/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
+++ b/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
@@ -585,7 +585,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="302">
   <si>
     <t>descr</t>
   </si>
@@ -1431,6 +1431,66 @@
   </si>
   <si>
     <t>Рассчитать минимальную партию для продажи или получить партию для продажи с учетом лимитов</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Выбрать целочисленное значение в процентах или абсолютное</t>
+  </si>
+  <si>
+    <t>Положительное - выбор в процентах; Отрицательное - выбор в абсолютных единицах; null - сбросить значение; $cGUI.Menu.Close - выбрано закрыть терминал; $cGUI.Menu.Back - выбрана опция возврата в предыдущее меню</t>
+  </si>
+  <si>
+    <t>Сформировать и отобразить меню, вернуть выбранную опцию.</t>
+  </si>
+  <si>
+    <t>Массив с опциями меню</t>
+  </si>
+  <si>
+    <t>Выбранное значение</t>
+  </si>
+  <si>
+    <t>Добавить в меню опцию редактирования целочисленного параметра, который может быть указан в единицах или процентах (MTB, MTS, etc...)</t>
+  </si>
+  <si>
+    <t>Текущее значение параметра</t>
+  </si>
+  <si>
+    <t>text-id краткого наименования опции</t>
+  </si>
+  <si>
+    <t>текстовый идентификатор опции, который должен быть возвращен в случае выбора в меню</t>
+  </si>
+  <si>
+    <t>text-id или текст тайтла меню (самая верхняя жирная строка)</t>
+  </si>
+  <si>
+    <t>text-id или текст с детальным описанием меню</t>
+  </si>
+  <si>
+    <t>text-id или текст краткого описания выбираемого значения (например: Мин. партия для покупки)</t>
+  </si>
+  <si>
+    <t>text-id или текст подробного описания значения (Например: Значение минимальной партии для покупки позволяет предотвратить рейсы…)</t>
+  </si>
+  <si>
+    <t>Выбрать цену товара</t>
+  </si>
+  <si>
+    <t>text-id или текст краткого описания выбираемого значения (например: Цена закупки)</t>
+  </si>
+  <si>
+    <t>Ware</t>
+  </si>
+  <si>
+    <t>Выбранная цена в пределах min-max цены товара; null - сбросить значение</t>
+  </si>
+  <si>
+    <t>Меню редактирование параметров товара</t>
+  </si>
+  <si>
+    <t>$cGUI.Menu.Close - выбрана опция закрытия терминала; $cGUI.Menu.Remove - выбрана опция удаления товара из списка; null - меню закрыто</t>
   </si>
 </sst>
 </file>
@@ -3575,11 +3635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K110"/>
+  <dimension ref="A1:K112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6372,60 +6432,150 @@
         <v>228</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A101" s="26"/>
-      <c r="B101" s="27"/>
-      <c r="C101" s="46"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="27"/>
-      <c r="F101" s="27"/>
-      <c r="G101" s="27"/>
-      <c r="H101" s="27"/>
-      <c r="I101" s="28"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A102" s="26"/>
-      <c r="B102" s="27"/>
-      <c r="C102" s="46"/>
-      <c r="D102" s="27"/>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="27"/>
-      <c r="H102" s="27"/>
-      <c r="I102" s="28"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="37"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="4"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A104" s="4"/>
-      <c r="B104" s="4"/>
-      <c r="C104" s="37"/>
-      <c r="D104" s="4"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A105" s="4"/>
-      <c r="B105" s="4"/>
-      <c r="C105" s="37"/>
-      <c r="D105" s="4"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4"/>
-      <c r="I105" s="4"/>
+    <row r="101" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="B101" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C101" s="46">
+        <v>12800</v>
+      </c>
+      <c r="D101" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="E101" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="F101" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="G101" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H101" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I101" s="28" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="B102" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C102" s="46">
+        <v>12801</v>
+      </c>
+      <c r="D102" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="E102" s="27" t="s">
+        <v>295</v>
+      </c>
+      <c r="F102" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G102" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H102" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I102" s="28" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B103" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C103" s="46">
+        <v>12802</v>
+      </c>
+      <c r="D103" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="E103" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="F103" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="G103" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="H103" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I103" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="B104" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C104" s="46">
+        <v>12803</v>
+      </c>
+      <c r="D104" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="E104" s="27" t="s">
+        <v>298</v>
+      </c>
+      <c r="F104" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G104" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H104" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I104" s="28" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="B105" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C105" s="46">
+        <v>12901</v>
+      </c>
+      <c r="D105" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="E105" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F105" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G105" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H105" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I105" s="28" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
@@ -6481,6 +6631,28 @@
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="37"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="4"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="37"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I60">
@@ -6506,7 +6678,7 @@
           <x14:formula1>
             <xm:f>Category!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1523</xm:sqref>
+          <xm:sqref>B2:B1525</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6516,7 +6688,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -6551,6 +6723,11 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
X3TC/T2D: New features and bugfixes
- WAL now works correctly on buying
- Added UI to spec. reserve setup
</commit_message>
<xml_diff>
--- a/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
+++ b/x3tc/T2-Droid/Documents/Readme.T2-Droid/wwsl-t2-function.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$114</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
@@ -522,7 +522,34 @@
         </r>
       </text>
     </comment>
-    <comment ref="F95" authorId="1">
+    <comment ref="K84" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Шалмеев Дмитрий:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+Медленная.
+См. 707 для быстрого отбора по main type ID</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F96" authorId="1">
       <text>
         <r>
           <rPr>
@@ -551,7 +578,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F96" authorId="1">
+    <comment ref="F97" authorId="1">
       <text>
         <r>
           <rPr>
@@ -585,7 +612,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="329">
   <si>
     <t>descr</t>
   </si>
@@ -1184,9 +1211,6 @@
     <t>Инициализировать структуру</t>
   </si>
   <si>
-    <t>Идентификатор структуры, одна из констант вида $const.STRUCT</t>
-  </si>
-  <si>
     <t>Экземпляр структуры</t>
   </si>
   <si>
@@ -1487,9 +1511,6 @@
     <t>Меню редактирование параметров товара</t>
   </si>
   <si>
-    <t>$cGUI.Menu.Close - выбрана опция закрытия терминала; $cGUI.Menu.Remove - выбрана опция удаления товара из списка; null - меню закрыто</t>
-  </si>
-  <si>
     <t>Количество батарей или 0, если пополнение не требуется.</t>
   </si>
   <si>
@@ -1518,6 +1539,66 @@
   </si>
   <si>
     <t>TRUE - есть прыжковый маяк</t>
+  </si>
+  <si>
+    <t>Меню редактирование спецрезерва</t>
+  </si>
+  <si>
+    <t>ShipStruct (опционально, если не указан, то конфигурация THIS)</t>
+  </si>
+  <si>
+    <t>Диалог выбора товара по main type</t>
+  </si>
+  <si>
+    <t>Main type</t>
+  </si>
+  <si>
+    <t>Получить список известных (has been discovered) товаров по main type</t>
+  </si>
+  <si>
+    <t>Список товаров</t>
+  </si>
+  <si>
+    <t>Массив товаров для исключения (опционально)</t>
+  </si>
+  <si>
+    <t>Флаги (опционально): 1 - включить equipment, 2 - включить upgrades</t>
+  </si>
+  <si>
+    <t>Main type ID (опционально)</t>
+  </si>
+  <si>
+    <t>Диалог выбора категории товара</t>
+  </si>
+  <si>
+    <t>Массив main type ID для включения</t>
+  </si>
+  <si>
+    <t>Main type ID - выбранная категория; $cGUI.Menu.Close - выбрана опция закрытия терминала; $cGUI.Menu.Back - меню закрыто</t>
+  </si>
+  <si>
+    <t>$cGUI.Menu.Close - выбрана опция закрытия терминала; $cGUI.Menu.Remove - выбрана опция удаления товара из списка; $cGUI.Menu.Back - меню закрыто</t>
+  </si>
+  <si>
+    <t>$cGUI.Menu.Close - выбрана опция закрытия терминала; $cGUI.Menu.Back - меню закрыто</t>
+  </si>
+  <si>
+    <t>Диалог выбора товара из списка</t>
+  </si>
+  <si>
+    <t>Массив товаров для выбора</t>
+  </si>
+  <si>
+    <t>Ware - выбранный товар; $cGUI.Menu.Close - выбрана опция закрытия терминала; $cGUI.Menu.Back - меню закрыто</t>
+  </si>
+  <si>
+    <t>Базовый text-id. Смещение +0 - menu heading, +1 - info line, +2 - title</t>
+  </si>
+  <si>
+    <t>Диалог выбора товара из указанных категорий</t>
+  </si>
+  <si>
+    <t>Идентификатор структуры, одна из констант</t>
   </si>
 </sst>
 </file>
@@ -1568,7 +1649,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1657,6 +1738,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor rgb="FFAECF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1750,7 +1837,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1869,6 +1956,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -3662,11 +3750,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:K120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K100" sqref="K100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3688,7 +3776,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>1</v>
@@ -3717,7 +3805,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C2" s="37">
         <v>1</v>
@@ -3743,14 +3831,14 @@
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="37">
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
@@ -3765,25 +3853,25 @@
         <v>10</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C4" s="37">
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>251</v>
-      </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
@@ -3794,26 +3882,26 @@
         <v>10</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C5" s="37">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>251</v>
-      </c>
       <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
@@ -3824,26 +3912,26 @@
         <v>10</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K5" s="24"/>
     </row>
     <row r="6" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C6" s="37">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>251</v>
-      </c>
       <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
@@ -3854,26 +3942,26 @@
         <v>10</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C7" s="37">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>251</v>
-      </c>
       <c r="F7" s="4" t="s">
         <v>10</v>
       </c>
@@ -3884,37 +3972,37 @@
         <v>10</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C8" s="37">
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>260</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>261</v>
       </c>
       <c r="K8" s="24"/>
     </row>
@@ -4004,7 +4092,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C12" s="37">
         <v>54</v>
@@ -4033,7 +4121,7 @@
         <v>27</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C13" s="37">
         <v>55</v>
@@ -4059,10 +4147,10 @@
     </row>
     <row r="14" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C14" s="37">
         <v>56</v>
@@ -4169,16 +4257,16 @@
     </row>
     <row r="18" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C18" s="37">
         <v>497</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>10</v>
@@ -4193,15 +4281,15 @@
         <v>10</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C19" s="37">
         <v>498</v>
@@ -4222,37 +4310,37 @@
         <v>10</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C20" s="37">
         <v>499</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>303</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>305</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>306</v>
       </c>
       <c r="K20" s="24"/>
     </row>
@@ -4366,16 +4454,16 @@
     </row>
     <row r="25" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C25" s="37">
         <v>504</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>10</v>
@@ -4390,7 +4478,7 @@
         <v>10</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K25" s="24"/>
     </row>
@@ -4418,7 +4506,7 @@
         <v>10</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="33" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4426,7 +4514,7 @@
         <v>57</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C27" s="43">
         <v>506</v>
@@ -4482,7 +4570,7 @@
         <v>62</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C29" s="42">
         <v>508</v>
@@ -4511,7 +4599,7 @@
         <v>65</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C30" s="37">
         <v>509</v>
@@ -4702,7 +4790,7 @@
         <v>80</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C37" s="37">
         <v>516</v>
@@ -4975,7 +5063,7 @@
     </row>
     <row r="47" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="37">
@@ -5264,35 +5352,35 @@
     </row>
     <row r="58" spans="1:11" s="16" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B58" s="15"/>
       <c r="C58" s="36">
         <v>601</v>
       </c>
       <c r="D58" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I58" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G58" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I58" s="15" t="s">
-        <v>236</v>
       </c>
       <c r="K58" s="24"/>
     </row>
     <row r="59" spans="1:11" s="16" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B59" s="15"/>
       <c r="C59" s="36">
@@ -5346,7 +5434,7 @@
     </row>
     <row r="61" spans="1:11" s="16" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B61" s="15"/>
       <c r="C61" s="36">
@@ -5374,7 +5462,7 @@
     </row>
     <row r="62" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B62" s="15"/>
       <c r="C62" s="36">
@@ -5484,14 +5572,14 @@
     </row>
     <row r="66" spans="1:11" s="16" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B66" s="15"/>
       <c r="C66" s="36">
         <v>609</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E66" s="15" t="s">
         <v>10</v>
@@ -5592,7 +5680,7 @@
     </row>
     <row r="70" spans="1:11" s="16" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B70" s="15"/>
       <c r="C70" s="36">
@@ -5948,7 +6036,7 @@
         <v>150</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C83" s="37">
         <v>700</v>
@@ -5972,12 +6060,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" ht="192" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>152</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C84" s="37">
         <v>701</v>
@@ -5992,7 +6080,7 @@
         <v>155</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H84" s="21" t="s">
         <v>10</v>
@@ -6000,12 +6088,15 @@
       <c r="I84" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="K84" s="48"/>
     </row>
     <row r="85" spans="1:11" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B85" s="4"/>
+      <c r="B85" s="4" t="s">
+        <v>271</v>
+      </c>
       <c r="C85" s="37">
         <v>702</v>
       </c>
@@ -6084,10 +6175,10 @@
     </row>
     <row r="88" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C88" s="37">
         <v>705</v>
@@ -6108,21 +6199,21 @@
         <v>10</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C89" s="37">
         <v>706</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>10</v>
@@ -6137,27 +6228,27 @@
         <v>10</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>198</v>
+        <v>313</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C90" s="37">
-        <v>8200</v>
+        <v>707</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>199</v>
+        <v>312</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>10</v>
+        <v>315</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>10</v>
+        <v>316</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>10</v>
@@ -6166,144 +6257,143 @@
         <v>10</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>200</v>
+        <v>314</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C91" s="37">
+        <v>8200</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="C91" s="37">
+      <c r="B92" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C92" s="37">
         <v>8201</v>
       </c>
-      <c r="D91" s="4" t="s">
+      <c r="D92" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I92" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="F91" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G91" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H91" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I91" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="26" t="s">
-        <v>196</v>
-      </c>
-      <c r="B92" s="27" t="s">
-        <v>268</v>
-      </c>
-      <c r="C92" s="46">
-        <v>8202</v>
-      </c>
-      <c r="D92" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="E92" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="F92" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="G92" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H92" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I92" s="28" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="B93" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="C93" s="46">
+        <v>8202</v>
+      </c>
+      <c r="D93" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E93" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="B93" s="27" t="s">
-        <v>268</v>
-      </c>
-      <c r="C93" s="46">
+      <c r="F93" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="G93" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I93" s="28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B94" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="C94" s="46">
         <v>8203</v>
       </c>
-      <c r="D93" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="E93" s="27" t="s">
+      <c r="D94" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E94" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="F94" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G94" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I94" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="F93" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G93" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H93" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I93" s="28" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="B94" s="27" t="s">
-        <v>268</v>
-      </c>
-      <c r="C94" s="46">
-        <v>8204</v>
-      </c>
-      <c r="D94" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="E94" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="F94" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G94" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H94" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I94" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="K94" s="24"/>
-    </row>
-    <row r="95" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="26" t="s">
         <v>243</v>
       </c>
       <c r="B95" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C95" s="46">
-        <v>8210</v>
+        <v>8204</v>
       </c>
       <c r="D95" s="27" t="s">
-        <v>200</v>
+        <v>245</v>
       </c>
       <c r="E95" s="27" t="s">
-        <v>210</v>
+        <v>244</v>
       </c>
       <c r="F95" s="27" t="s">
-        <v>242</v>
+        <v>10</v>
       </c>
       <c r="G95" s="27" t="s">
         <v>10</v>
@@ -6312,86 +6402,87 @@
         <v>10</v>
       </c>
       <c r="I95" s="28" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="K95" s="24"/>
     </row>
     <row r="96" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="26" t="s">
-        <v>202</v>
+        <v>242</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C96" s="46">
-        <v>8211</v>
+        <v>8210</v>
       </c>
       <c r="D96" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="F96" s="27" t="s">
-        <v>204</v>
+        <v>241</v>
       </c>
       <c r="G96" s="27" t="s">
-        <v>237</v>
+        <v>10</v>
       </c>
       <c r="H96" s="27" t="s">
         <v>10</v>
       </c>
       <c r="I96" s="28" t="s">
-        <v>205</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="K96" s="24"/>
     </row>
     <row r="97" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="26" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B97" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C97" s="46">
-        <v>8212</v>
+        <v>8211</v>
       </c>
       <c r="D97" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E97" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="F97" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="F97" s="27" t="s">
-        <v>206</v>
-      </c>
       <c r="G97" s="27" t="s">
-        <v>10</v>
+        <v>236</v>
       </c>
       <c r="H97" s="27" t="s">
         <v>10</v>
       </c>
       <c r="I97" s="28" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="26" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B98" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C98" s="46">
-        <v>8213</v>
+        <v>8212</v>
       </c>
       <c r="D98" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E98" s="27" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F98" s="27" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="G98" s="27" t="s">
         <v>10</v>
@@ -6400,28 +6491,28 @@
         <v>10</v>
       </c>
       <c r="I98" s="28" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="26" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B99" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C99" s="46">
-        <v>8214</v>
+        <v>8213</v>
       </c>
       <c r="D99" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E99" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="F99" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="F99" s="27" t="s">
-        <v>10</v>
-      </c>
       <c r="G99" s="27" t="s">
         <v>10</v>
       </c>
@@ -6429,26 +6520,26 @@
         <v>10</v>
       </c>
       <c r="I99" s="28" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="26" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B100" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C100" s="46">
-        <v>8215</v>
+        <v>8214</v>
       </c>
       <c r="D100" s="27" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="E100" s="27" t="s">
-        <v>210</v>
-      </c>
-      <c r="F100" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="F100" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G100" s="27" t="s">
@@ -6458,27 +6549,27 @@
         <v>10</v>
       </c>
       <c r="I100" s="28" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="26" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B101" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C101" s="46">
-        <v>8221</v>
+        <v>8215</v>
       </c>
       <c r="D101" s="27" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
       <c r="E101" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="F101" s="34" t="s">
-        <v>224</v>
+        <v>209</v>
+      </c>
+      <c r="F101" s="29" t="s">
+        <v>10</v>
       </c>
       <c r="G101" s="27" t="s">
         <v>10</v>
@@ -6487,24 +6578,24 @@
         <v>10</v>
       </c>
       <c r="I101" s="28" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="26" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B102" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C102" s="46">
-        <v>8222</v>
+        <v>8221</v>
       </c>
       <c r="D102" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E102" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F102" s="34" t="s">
         <v>223</v>
@@ -6516,248 +6607,356 @@
         <v>10</v>
       </c>
       <c r="I102" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="26" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B103" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C103" s="46">
-        <v>8223</v>
+        <v>8222</v>
       </c>
       <c r="D103" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E103" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="F103" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="G103" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H103" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I103" s="28" t="s">
         <v>213</v>
-      </c>
-      <c r="F103" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="G103" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H103" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I103" s="28" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="B104" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="C104" s="46">
+        <v>8223</v>
+      </c>
+      <c r="D104" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E104" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="F104" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="G104" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H104" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I104" s="28" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="B105" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C105" s="46">
+        <v>12800</v>
+      </c>
+      <c r="D105" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B104" s="27" t="s">
+      <c r="E105" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="F105" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="G105" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H105" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I105" s="28" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="26" t="s">
         <v>281</v>
       </c>
-      <c r="C104" s="46">
-        <v>12800</v>
-      </c>
-      <c r="D104" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="E104" s="27" t="s">
-        <v>291</v>
-      </c>
-      <c r="F104" s="27" t="s">
+      <c r="B106" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C106" s="46">
+        <v>12801</v>
+      </c>
+      <c r="D106" s="27" t="s">
         <v>292</v>
       </c>
-      <c r="G104" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H104" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I104" s="28" t="s">
+      <c r="E106" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="F106" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G106" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H106" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I106" s="28" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="26" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="26" t="s">
-        <v>282</v>
-      </c>
-      <c r="B105" s="27" t="s">
-        <v>281</v>
-      </c>
-      <c r="C105" s="46">
-        <v>12801</v>
-      </c>
-      <c r="D105" s="27" t="s">
-        <v>293</v>
-      </c>
-      <c r="E105" s="27" t="s">
-        <v>294</v>
-      </c>
-      <c r="F105" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G105" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H105" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I105" s="28" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="26" t="s">
+      <c r="B107" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C107" s="46">
+        <v>12802</v>
+      </c>
+      <c r="D107" s="27" t="s">
+        <v>284</v>
+      </c>
+      <c r="E107" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="B106" s="27" t="s">
-        <v>281</v>
-      </c>
-      <c r="C106" s="46">
-        <v>12802</v>
-      </c>
-      <c r="D106" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="E106" s="27" t="s">
+      <c r="F107" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="F106" s="27" t="s">
+      <c r="G107" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="G106" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="H106" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I106" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="B107" s="27" t="s">
-        <v>281</v>
-      </c>
-      <c r="C107" s="46">
-        <v>12803</v>
-      </c>
-      <c r="D107" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="E107" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="F107" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G107" s="27" t="s">
-        <v>10</v>
-      </c>
       <c r="H107" s="27" t="s">
         <v>10</v>
       </c>
       <c r="I107" s="28" t="s">
-        <v>298</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="26" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B108" s="27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C108" s="46">
+        <v>12803</v>
+      </c>
+      <c r="D108" s="27" t="s">
+        <v>295</v>
+      </c>
+      <c r="E108" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="F108" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G108" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H108" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I108" s="28" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="B109" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C109" s="46">
+        <v>12804</v>
+      </c>
+      <c r="D109" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="E109" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="G109" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H109" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I109" s="28" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="B110" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C110" s="46">
+        <v>12805</v>
+      </c>
+      <c r="D110" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="G110" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H110" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I110" s="28" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="B111" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C111" s="46">
+        <v>12806</v>
+      </c>
+      <c r="D111" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="E111" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="F111" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G111" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H111" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I111" s="28" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="B112" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C112" s="46">
+        <v>12807</v>
+      </c>
+      <c r="D112" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="E112" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="F112" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="G112" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H112" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I112" s="28" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="B113" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C113" s="46">
         <v>12901</v>
       </c>
-      <c r="D108" s="27" t="s">
+      <c r="D113" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="E108" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F108" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G108" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H108" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I108" s="28" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="37"/>
-      <c r="D109" s="4"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="4"/>
-      <c r="G109" s="4"/>
-      <c r="H109" s="4"/>
-      <c r="I109" s="4"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="4"/>
-      <c r="B110" s="4"/>
-      <c r="C110" s="37"/>
-      <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
-      <c r="I110" s="4"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A111" s="4"/>
-      <c r="B111" s="4"/>
-      <c r="C111" s="37"/>
-      <c r="D111" s="4"/>
-      <c r="E111" s="4"/>
-      <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
-      <c r="H111" s="4"/>
-      <c r="I111" s="4"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A112" s="4"/>
-      <c r="B112" s="4"/>
-      <c r="C112" s="37"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="4"/>
-      <c r="G112" s="4"/>
-      <c r="H112" s="4"/>
-      <c r="I112" s="4"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" s="4"/>
-      <c r="B113" s="4"/>
-      <c r="C113" s="37"/>
-      <c r="D113" s="4"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="4"/>
-      <c r="G113" s="4"/>
-      <c r="H113" s="4"/>
-      <c r="I113" s="4"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A114" s="4"/>
-      <c r="B114" s="4"/>
-      <c r="C114" s="37"/>
-      <c r="D114" s="4"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="4"/>
-      <c r="G114" s="4"/>
-      <c r="H114" s="4"/>
-      <c r="I114" s="4"/>
+      <c r="E113" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G113" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H113" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I113" s="28" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="B114" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C114" s="46">
+        <v>12902</v>
+      </c>
+      <c r="D114" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="E114" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F114" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G114" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H114" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I114" s="28" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="4"/>
@@ -6770,8 +6969,63 @@
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
     </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="37"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
+      <c r="I116" s="4"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="37"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="4"/>
+      <c r="G117" s="4"/>
+      <c r="H117" s="4"/>
+      <c r="I117" s="4"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="37"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="4"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="37"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="4"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="37"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I63">
+  <autoFilter ref="A1:I114">
     <sortState ref="A2:I100">
       <sortCondition ref="C1:C60"/>
     </sortState>
@@ -6794,7 +7048,7 @@
           <x14:formula1>
             <xm:f>Category!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1528</xm:sqref>
+          <xm:sqref>B2:B1533</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6818,37 +7072,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>